<commit_message>
refact: update KYCProfile attributes
</commit_message>
<xml_diff>
--- a/src/app/modules/kyc/kyc_models/MVP-2-KYC-Commons-41.xlsx
+++ b/src/app/modules/kyc/kyc_models/MVP-2-KYC-Commons-41.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="309">
   <si>
     <t xml:space="preserve">Processus d’inscription : éléments communs et différenciants</t>
   </si>
@@ -391,7 +391,7 @@
     <t xml:space="preserve">Métier</t>
   </si>
   <si>
-    <t xml:space="preserve">metier1</t>
+    <t xml:space="preserve">metier_principal</t>
   </si>
   <si>
     <t xml:space="preserve">(multiple)  ONTOLOGIES/Métiers</t>
@@ -1014,6 +1014,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">trigger_media_media</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1047,6 +1050,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">trigger_media_federation</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1152,6 +1158,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">trigger_pr_organisation</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1185,7 +1194,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">trigger_organization</t>
+    <t xml:space="preserve">trigger_organisation</t>
   </si>
   <si>
     <r>
@@ -1221,6 +1230,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">trigger_expert</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1252,6 +1264,9 @@
       </rPr>
       <t xml:space="preserve">&lt;/strong&gt;. Vous pourrez étendre votre sphère d’influence et accroître vos revenus en acquérant de nouveaux clients ainsi que de nouveaux partenaires. Cochez la case ci-contre pour découvrir tous les avantages exclusifs que vous méritez.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">trigger_startup</t>
   </si>
   <si>
     <r>
@@ -2118,10 +2133,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="13412" ySplit="0" topLeftCell="G4" activePane="topRight" state="split"/>
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="topRight" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="13412" ySplit="0" topLeftCell="H74" activePane="topRight" state="split"/>
+      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
+      <selection pane="topRight" activeCell="I76" activeCellId="0" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6304,7 +6319,7 @@
       <c r="AQ67" s="6"/>
       <c r="AR67" s="6"/>
     </row>
-    <row r="68" customFormat="false" ht="46.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="46.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="45" t="s">
         <v>281</v>
       </c>
@@ -6314,8 +6329,12 @@
       <c r="E68" s="3"/>
       <c r="F68" s="45"/>
       <c r="G68" s="42"/>
-      <c r="H68" s="45"/>
-      <c r="I68" s="62"/>
+      <c r="H68" s="45" t="s">
+        <v>282</v>
+      </c>
+      <c r="I68" s="62" t="s">
+        <v>270</v>
+      </c>
       <c r="J68" s="62"/>
       <c r="K68" s="62"/>
       <c r="L68" s="6"/>
@@ -6352,9 +6371,9 @@
       <c r="AQ68" s="6"/>
       <c r="AR68" s="6"/>
     </row>
-    <row r="69" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="68.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="45" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B69" s="45"/>
       <c r="C69" s="45"/>
@@ -6362,8 +6381,12 @@
       <c r="E69" s="3"/>
       <c r="F69" s="45"/>
       <c r="G69" s="42"/>
-      <c r="H69" s="45"/>
-      <c r="I69" s="62"/>
+      <c r="H69" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="I69" s="62" t="s">
+        <v>270</v>
+      </c>
       <c r="J69" s="62"/>
       <c r="K69" s="62"/>
       <c r="L69" s="6"/>
@@ -6402,7 +6425,7 @@
     </row>
     <row r="70" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="63" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -6413,7 +6436,7 @@
       <c r="F70" s="3"/>
       <c r="G70" s="42"/>
       <c r="H70" s="45" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="I70" s="62" t="s">
         <v>270</v>
@@ -6456,7 +6479,7 @@
     </row>
     <row r="71" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="63" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -6467,7 +6490,7 @@
       <c r="F71" s="3"/>
       <c r="G71" s="42"/>
       <c r="H71" s="45" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="I71" s="62" t="s">
         <v>270</v>
@@ -6508,9 +6531,9 @@
       <c r="AQ71" s="6"/>
       <c r="AR71" s="6"/>
     </row>
-    <row r="72" customFormat="false" ht="70.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="70.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="63" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -6518,8 +6541,12 @@
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="42"/>
-      <c r="H72" s="45"/>
-      <c r="I72" s="62"/>
+      <c r="H72" s="45" t="s">
+        <v>290</v>
+      </c>
+      <c r="I72" s="62" t="s">
+        <v>270</v>
+      </c>
       <c r="J72" s="62"/>
       <c r="K72" s="62"/>
       <c r="L72" s="6"/>
@@ -6558,7 +6585,7 @@
     </row>
     <row r="73" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="63" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -6569,7 +6596,7 @@
       <c r="F73" s="3"/>
       <c r="G73" s="42"/>
       <c r="H73" s="45" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="I73" s="62" t="s">
         <v>270</v>
@@ -6610,9 +6637,9 @@
       <c r="AQ73" s="6"/>
       <c r="AR73" s="6"/>
     </row>
-    <row r="74" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="55.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="63" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -6620,8 +6647,12 @@
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="42"/>
-      <c r="H74" s="45"/>
-      <c r="I74" s="62"/>
+      <c r="H74" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="I74" s="62" t="s">
+        <v>270</v>
+      </c>
       <c r="J74" s="62"/>
       <c r="K74" s="62"/>
       <c r="L74" s="6"/>
@@ -6658,9 +6689,9 @@
       <c r="AQ74" s="6"/>
       <c r="AR74" s="6"/>
     </row>
-    <row r="75" customFormat="false" ht="46.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="46.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="45" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -6668,8 +6699,12 @@
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="42"/>
-      <c r="H75" s="45"/>
-      <c r="I75" s="62"/>
+      <c r="H75" s="45" t="s">
+        <v>296</v>
+      </c>
+      <c r="I75" s="62" t="s">
+        <v>270</v>
+      </c>
       <c r="J75" s="62"/>
       <c r="K75" s="62"/>
       <c r="L75" s="6"/>
@@ -6708,7 +6743,7 @@
     </row>
     <row r="76" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="63" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="B76" s="45"/>
       <c r="C76" s="45"/>
@@ -6719,7 +6754,7 @@
       <c r="F76" s="45"/>
       <c r="G76" s="42"/>
       <c r="H76" s="45" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="I76" s="62" t="s">
         <v>270</v>
@@ -6762,7 +6797,7 @@
     </row>
     <row r="77" customFormat="false" ht="69.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="63" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="B77" s="45"/>
       <c r="C77" s="45"/>
@@ -6773,7 +6808,7 @@
       <c r="F77" s="45"/>
       <c r="G77" s="42"/>
       <c r="H77" s="45" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="I77" s="62" t="s">
         <v>270</v>
@@ -6816,7 +6851,7 @@
     </row>
     <row r="78" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="63" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="B78" s="45"/>
       <c r="C78" s="45"/>
@@ -6827,7 +6862,7 @@
       <c r="F78" s="45"/>
       <c r="G78" s="42"/>
       <c r="H78" s="45" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="I78" s="62" t="s">
         <v>270</v>
@@ -6870,7 +6905,7 @@
     </row>
     <row r="79" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="63" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="B79" s="45"/>
       <c r="C79" s="45"/>
@@ -6881,7 +6916,7 @@
       <c r="F79" s="45"/>
       <c r="G79" s="42"/>
       <c r="H79" s="45" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="I79" s="62" t="s">
         <v>270</v>
@@ -6924,7 +6959,7 @@
     </row>
     <row r="80" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="B80" s="28"/>
       <c r="C80" s="28"/>
@@ -6974,7 +7009,7 @@
     </row>
     <row r="81" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="45" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -6983,10 +7018,10 @@
       <c r="F81" s="3"/>
       <c r="G81" s="42"/>
       <c r="H81" s="45" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="I81" s="62" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="J81" s="62"/>
       <c r="K81" s="62"/>

</xml_diff>

<commit_message>
fix: metier_principal not found in User class, add method KYCProfile.has_field_name()
</commit_message>
<xml_diff>
--- a/src/app/modules/kyc/kyc_models/MVP-2-KYC-Commons-41.xlsx
+++ b/src/app/modules/kyc/kyc_models/MVP-2-KYC-Commons-41.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="309">
   <si>
     <t xml:space="preserve">Processus d’inscription : éléments communs et différenciants</t>
   </si>
@@ -2133,10 +2133,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="13412" ySplit="0" topLeftCell="H74" activePane="topRight" state="split"/>
-      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
-      <selection pane="topRight" activeCell="I76" activeCellId="0" sqref="I76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="11187" ySplit="0" topLeftCell="C58" activePane="topRight" state="split"/>
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+      <selection pane="topRight" activeCell="E75" activeCellId="0" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6326,7 +6326,9 @@
       <c r="B68" s="45"/>
       <c r="C68" s="45"/>
       <c r="D68" s="45"/>
-      <c r="E68" s="3"/>
+      <c r="E68" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="F68" s="45"/>
       <c r="G68" s="42"/>
       <c r="H68" s="45" t="s">
@@ -6378,7 +6380,9 @@
       <c r="B69" s="45"/>
       <c r="C69" s="45"/>
       <c r="D69" s="45"/>
-      <c r="E69" s="3"/>
+      <c r="E69" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="F69" s="45"/>
       <c r="G69" s="42"/>
       <c r="H69" s="45" t="s">
@@ -6538,7 +6542,9 @@
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
+      <c r="E72" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="F72" s="3"/>
       <c r="G72" s="42"/>
       <c r="H72" s="45" t="s">
@@ -6644,7 +6650,9 @@
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
+      <c r="E74" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="F74" s="3"/>
       <c r="G74" s="42"/>
       <c r="H74" s="45" t="s">
@@ -6696,7 +6704,9 @@
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
+      <c r="E75" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="F75" s="3"/>
       <c r="G75" s="42"/>
       <c r="H75" s="45" t="s">

</xml_diff>